<commit_message>
update relationships & files
</commit_message>
<xml_diff>
--- a/output/frat/depth_1/frat_3_conceptnet_search.xlsx
+++ b/output/frat/depth_1/frat_3_conceptnet_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\r_m_thesis\output\frat\depth_1\updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rejna/projects/github.com/r_m_thesis/output/frat/depth_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FFC03E-0DD4-442A-BA8F-B3718C78A21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46E758C-E1DD-8444-9340-9AA7A073CEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19100" yWindow="11670" windowWidth="9820" windowHeight="5220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28980" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -628,15 +628,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="5" max="5" width="93.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="93.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -682,7 +682,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -702,7 +702,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -722,7 +722,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -742,7 +742,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -762,7 +762,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -782,7 +782,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -802,7 +802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -822,7 +822,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -842,7 +842,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -862,7 +862,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -882,7 +882,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -902,7 +902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H14" t="s">
         <v>66</v>
       </c>

</xml_diff>